<commit_message>
Cambios extra: versión 1
</commit_message>
<xml_diff>
--- a/estadisticas_jugador.xlsx
+++ b/estadisticas_jugador.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +506,98 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Solitario</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Annabmota</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>209</v>
+      </c>
+      <c r="D4" t="n">
+        <v>9</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-11-06 19:21:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Multijugador</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Jimena</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>283</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-11-06 19:34:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Solitario</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Annita</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>834</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-11-06 19:40:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Solitario</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Prueba</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>516</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2025-11-06 19:53:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambios extra: versión 4 (introducir validar números en multijugador)
</commit_message>
<xml_diff>
--- a/estadisticas_jugador.xlsx
+++ b/estadisticas_jugador.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -667,6 +667,29 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Solitario</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Anna</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>502</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2025-11-08 20:50:26</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambios extra: versión 5
</commit_message>
<xml_diff>
--- a/estadisticas_jugador.xlsx
+++ b/estadisticas_jugador.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -690,6 +690,52 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Solitario</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Ulises el amor de mi vida</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>732</v>
+      </c>
+      <c r="D12" t="n">
+        <v>12</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2025-11-11 00:29:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Multijugador</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Guillermina</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>283</v>
+      </c>
+      <c r="D13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2025-11-11 00:30:29</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Entrega final v2: terminada
</commit_message>
<xml_diff>
--- a/estadisticas_jugador.xlsx
+++ b/estadisticas_jugador.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,107 +473,23 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Anna</t>
+          <t>Ulises</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>283</v>
+        <v>395</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Victoria</t>
+          <t>Derrota</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-11-24 21:30:44</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Solitario</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Tonto</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>549</v>
-      </c>
-      <c r="D3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Derrota</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-11-24 21:38:56</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Solitario</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Anna</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>838</v>
-      </c>
-      <c r="D4" t="n">
-        <v>11</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Victoria</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-11-24 21:41:51</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Multijugador</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Uli</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>192</v>
-      </c>
-      <c r="D5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Victoria</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2025-11-24 21:42:11</t>
+          <t>2025-11-24 21:51:16</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Entrega final: versión 3
</commit_message>
<xml_diff>
--- a/estadisticas_jugador.xlsx
+++ b/estadisticas_jugador.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,28 +468,164 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Solitario</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Annabelle</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>190</v>
+      </c>
+      <c r="D2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Victoria</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-26 15:26:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Solitario</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>288</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Victoria</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-11-26 15:27:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Solitario</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Annabelle</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>348</v>
+      </c>
+      <c r="D4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Victoria</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-11-26 15:43:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Solitario</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Ulises</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>795</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Derrota</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-11-26 15:43:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>Multijugador</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Ulises</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>395</v>
-      </c>
-      <c r="D2" t="n">
-        <v>5</v>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Uli</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>192</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Victoria</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-11-26 15:55:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Multijugador</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Pepe</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>923</v>
+      </c>
+      <c r="D7" t="n">
+        <v>12</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>Derrota</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2025-11-24 21:51:16</t>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-11-26 15:56:40</t>
         </is>
       </c>
     </row>

</xml_diff>